<commit_message>
Updated path to dropbox
</commit_message>
<xml_diff>
--- a/Points.xlsx
+++ b/Points.xlsx
@@ -1,119 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\19-09-24 Yiffy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8356BEB-DD11-480E-B176-362F710A915C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Team_Id</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Oren's Team</t>
-  </si>
-  <si>
-    <t>13 Cups</t>
-  </si>
-  <si>
-    <t>Chris's Team</t>
-  </si>
-  <si>
-    <t>Cosminutz</t>
-  </si>
-  <si>
-    <t>Dropping The Gloves</t>
-  </si>
-  <si>
-    <t>Klin Krush</t>
-  </si>
-  <si>
-    <t>Nylanderthal</t>
-  </si>
-  <si>
-    <t>RUXANDRA's Team</t>
-  </si>
-  <si>
-    <t>Stacey's Superb Team</t>
-  </si>
-  <si>
-    <t>The Black Swans</t>
-  </si>
-  <si>
-    <t>TJ Team</t>
-  </si>
-  <si>
-    <t>Unty's Assassins</t>
-  </si>
-  <si>
-    <t>Yani's Team</t>
-  </si>
-  <si>
-    <t>The Mighty Pigs</t>
-  </si>
-  <si>
-    <t>Jon's Team</t>
-  </si>
-  <si>
-    <t>Thomas's Team</t>
-  </si>
-  <si>
-    <t>Jarrod's Team</t>
-  </si>
-  <si>
-    <t>Benchwarmers</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -129,36 +59,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -458,139 +379,305 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="19" width="14.140625" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="8.5703125"/>
+    <col customWidth="1" max="19" min="2" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Team_Id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="P1" s="3">
+      <c r="P1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="Q1" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="R1" s="3">
+      <c r="R1" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="S1" s="3">
+      <c r="S1" s="3" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>19</v>
+    <row customHeight="1" ht="49.5" r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Oren's Team</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>13 Cups</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Chris's Team</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Cosminutz</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Dropping The Gloves</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>Klin Krush</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>Nylanderthal</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>RUXANDRA's Team</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>Stacey's Superb Team</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>The Black Swans</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>TJ Team</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>Unty's Assassins</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>Yani's Team</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>The Mighty Pigs</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>Jon's Team</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>Thomas's Team</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>Jarrod's Team</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>Benchwarmers</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>25/09/2019</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>26/09/2019</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added iPython notebook and changed team id from string to int
</commit_message>
<xml_diff>
--- a/Points.xlsx
+++ b/Points.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\yffpy-batch\fantasy-points\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DD58FA-44BD-47CE-B79D-04F6C7F376BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{361A9422-F73F-4DA2-827A-880802CFA75C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,10 +82,10 @@
     <t>Benchwarmers</t>
   </si>
   <si>
-    <t>25/09/2019</t>
-  </si>
-  <si>
-    <t>26/09/2019</t>
+    <t>Air Duct Cleaners</t>
+  </si>
+  <si>
+    <t>03/10/2019</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -151,6 +151,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,19 +469,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A6" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="19" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,8 +539,11 @@
       <c r="S1" s="3">
         <v>18</v>
       </c>
+      <c r="T1" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -594,10 +601,13 @@
       <c r="S2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="T2" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>43740</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -653,64 +663,70 @@
       <c r="S3">
         <v>0</v>
       </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>6.7</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>11.2</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>14.25</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>11.25</v>
+      </c>
+      <c r="T4">
+        <v>9.1999999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>